<commit_message>
Add timesheet records including pitch presentation, business case and mileston plan
</commit_message>
<xml_diff>
--- a/Time sheet/Timetsheet - Eric(Week2).xlsx
+++ b/Time sheet/Timetsheet - Eric(Week2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/Google Drive/U Adelaide course materials/MCI projects/Team-024/Time sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2826F271-E5CC-EA44-B223-10343F4F4697}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C6733A-E71B-0444-861E-C039D71EB3D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -259,7 +259,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -314,6 +314,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -661,7 +664,7 @@
   <dimension ref="A2:AW12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -797,7 +800,9 @@
       <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="21">
+        <v>44264</v>
+      </c>
       <c r="C7" s="19">
         <v>0.375</v>
       </c>
@@ -915,11 +920,13 @@
       <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="16">
+      <c r="B9" s="21">
+        <v>44266</v>
+      </c>
+      <c r="C9" s="19">
         <v>0.5</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="19">
         <v>0.75</v>
       </c>
       <c r="E9" s="12">

</xml_diff>